<commit_message>
Add configuration for m/m/1
</commit_message>
<xml_diff>
--- a/2k factorial.xlsx
+++ b/2k factorial.xlsx
@@ -9,12 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="28800" yWindow="0" windowWidth="38400" windowHeight="21600" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16000" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Arkusz1" sheetId="1" r:id="rId1"/>
-    <sheet name="Arkusz2" sheetId="2" r:id="rId2"/>
-    <sheet name="Arkusz3" sheetId="3" r:id="rId3"/>
+    <sheet name="Arkusz4" sheetId="4" r:id="rId2"/>
+    <sheet name="Arkusz2" sheetId="2" r:id="rId3"/>
+    <sheet name="Arkusz3" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
@@ -416,10 +417,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S18"/>
+  <dimension ref="A1:X18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H3" sqref="H3:J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -428,7 +429,7 @@
     <col min="15" max="15" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.2">
       <c r="C1" t="s">
         <v>4</v>
       </c>
@@ -436,7 +437,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
         <v>3</v>
       </c>
@@ -450,7 +451,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -469,43 +470,55 @@
       </c>
       <c r="F3">
         <f t="shared" ref="F3:F5" si="0">SUM(H3:J3)/3</f>
-        <v>12830.333333333334</v>
+        <v>4.1082194404051471</v>
       </c>
       <c r="H3">
-        <v>12833</v>
+        <v>4.1083281942661838</v>
       </c>
       <c r="I3">
-        <v>12684</v>
+        <v>4.1032562333550509</v>
       </c>
       <c r="J3">
-        <v>12974</v>
+        <v>4.1130738935942075</v>
       </c>
       <c r="L3">
         <f>H3-$F3</f>
-        <v>2.6666666666660603</v>
+        <v>1.0875386103670337E-4</v>
       </c>
       <c r="M3">
         <f t="shared" ref="M3:N3" si="1">I3-$F3</f>
-        <v>-146.33333333333394</v>
+        <v>-4.96320705009623E-3</v>
       </c>
       <c r="N3">
         <f t="shared" si="1"/>
-        <v>143.66666666666606</v>
+        <v>4.8544531890604148E-3</v>
       </c>
       <c r="P3">
         <f>L3^2</f>
-        <v>7.1111111111078777</v>
+        <v>1.1827402290390588E-8</v>
       </c>
       <c r="Q3">
-        <f t="shared" ref="Q3:R3" si="2">M3^2</f>
-        <v>21413.444444444624</v>
+        <f>M3^2</f>
+        <v>2.463342422212492E-5</v>
       </c>
       <c r="R3">
-        <f t="shared" si="2"/>
-        <v>20640.111111110939</v>
-      </c>
-    </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.2">
+        <f t="shared" ref="Q3:R3" si="2">N3^2</f>
+        <v>2.3565715764778833E-5</v>
+      </c>
+      <c r="U3">
+        <f>(H3-$J$8)^2</f>
+        <v>8.2304076012970271E-4</v>
+      </c>
+      <c r="V3">
+        <f t="shared" ref="V3:W3" si="3">(I3-$J$8)^2</f>
+        <v>5.5774974979477083E-4</v>
+      </c>
+      <c r="W3">
+        <f t="shared" si="3"/>
+        <v>1.1178581872036228E-3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -519,48 +532,60 @@
         <v>-1</v>
       </c>
       <c r="E4">
-        <f t="shared" ref="E4:E6" si="3">C4*D4</f>
+        <f t="shared" ref="E4:E6" si="4">C4*D4</f>
         <v>-1</v>
       </c>
       <c r="F4">
         <f t="shared" si="0"/>
-        <v>12297</v>
+        <v>4.0896631400559587</v>
       </c>
       <c r="H4">
-        <v>12732</v>
+        <v>4.1048966299489651</v>
       </c>
       <c r="I4">
-        <v>12038</v>
+        <v>4.0805543389887715</v>
       </c>
       <c r="J4">
-        <v>12121</v>
+        <v>4.0835384512301394</v>
       </c>
       <c r="L4">
-        <f t="shared" ref="L4:L6" si="4">H4-$F4</f>
-        <v>435</v>
+        <f t="shared" ref="L4:L6" si="5">H4-$F4</f>
+        <v>1.5233489893006436E-2</v>
       </c>
       <c r="M4">
-        <f t="shared" ref="M4:M6" si="5">I4-$F4</f>
-        <v>-259</v>
+        <f t="shared" ref="M4:M6" si="6">I4-$F4</f>
+        <v>-9.1088010671871444E-3</v>
       </c>
       <c r="N4">
-        <f t="shared" ref="N4:N6" si="6">J4-$F4</f>
-        <v>-176</v>
+        <f t="shared" ref="N4:N6" si="7">J4-$F4</f>
+        <v>-6.1246888258192911E-3</v>
       </c>
       <c r="P4">
-        <f t="shared" ref="P4:P6" si="7">L4^2</f>
-        <v>189225</v>
+        <f t="shared" ref="P4:P6" si="8">L4^2</f>
+        <v>2.3205921432032923E-4</v>
       </c>
       <c r="Q4">
-        <f t="shared" ref="Q4:Q6" si="8">M4^2</f>
-        <v>67081</v>
+        <f t="shared" ref="Q4:Q6" si="9">M4^2</f>
+        <v>8.2970256881589663E-5</v>
       </c>
       <c r="R4">
-        <f t="shared" ref="R4:R6" si="9">N4^2</f>
-        <v>30976</v>
-      </c>
-    </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.2">
+        <f t="shared" ref="R4:R6" si="10">N4^2</f>
+        <v>3.751181321311569E-5</v>
+      </c>
+      <c r="U4">
+        <f t="shared" ref="U4:U6" si="11">(H4-$J$8)^2</f>
+        <v>6.379222447566728E-4</v>
+      </c>
+      <c r="V4">
+        <f t="shared" ref="V4:V6" si="12">(I4-$J$8)^2</f>
+        <v>8.3691702790118622E-7</v>
+      </c>
+      <c r="W4">
+        <f t="shared" ref="W4:W6" si="13">(J4-$J$8)^2</f>
+        <v>1.5201763809242125E-5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -574,48 +599,60 @@
         <v>1</v>
       </c>
       <c r="E5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>-1</v>
       </c>
       <c r="F5">
         <f t="shared" si="0"/>
-        <v>12446.666666666666</v>
+        <v>4.0949824989858037</v>
       </c>
       <c r="H5">
-        <v>12140</v>
+        <v>4.0842186867392387</v>
       </c>
       <c r="I5">
-        <v>12667</v>
+        <v>4.1026737705489271</v>
       </c>
       <c r="J5">
-        <v>12533</v>
+        <v>4.0980550396692434</v>
       </c>
       <c r="L5">
-        <f t="shared" si="4"/>
-        <v>-306.66666666666606</v>
+        <f t="shared" si="5"/>
+        <v>-1.0763812246564974E-2</v>
       </c>
       <c r="M5">
-        <f t="shared" si="5"/>
-        <v>220.33333333333394</v>
+        <f t="shared" si="6"/>
+        <v>7.6912715631234363E-3</v>
       </c>
       <c r="N5">
-        <f t="shared" si="6"/>
-        <v>86.33333333333394</v>
+        <f t="shared" si="7"/>
+        <v>3.0725406834397617E-3</v>
       </c>
       <c r="P5">
-        <f t="shared" si="7"/>
-        <v>94044.444444444074</v>
+        <f t="shared" si="8"/>
+        <v>1.1585965407930212E-4</v>
       </c>
       <c r="Q5">
-        <f t="shared" si="8"/>
-        <v>48546.777777778043</v>
+        <f t="shared" si="9"/>
+        <v>5.915565825771123E-5</v>
       </c>
       <c r="R5">
-        <f t="shared" si="9"/>
-        <v>7453.4444444445489</v>
-      </c>
-    </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.2">
+        <f t="shared" si="10"/>
+        <v>9.4405062513924774E-6</v>
+      </c>
+      <c r="U5">
+        <f t="shared" si="11"/>
+        <v>2.0968884382399876E-5</v>
+      </c>
+      <c r="V5">
+        <f t="shared" si="12"/>
+        <v>5.3057728365052067E-4</v>
+      </c>
+      <c r="W5">
+        <f t="shared" si="13"/>
+        <v>3.3913183262625159E-4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>8</v>
       </c>
@@ -629,181 +666,201 @@
         <v>1</v>
       </c>
       <c r="E6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="F6">
         <f>SUM(H6:J6)/3</f>
-        <v>10615.666666666666</v>
+        <v>4.0256929497331528</v>
       </c>
       <c r="H6">
-        <v>10582</v>
+        <v>4.0245677571960377</v>
       </c>
       <c r="I6">
-        <v>11077</v>
+        <v>4.0444221557118434</v>
       </c>
       <c r="J6">
-        <v>10188</v>
+        <v>4.0080889362915775</v>
       </c>
       <c r="L6">
-        <f t="shared" si="4"/>
-        <v>-33.66666666666606</v>
+        <f t="shared" si="5"/>
+        <v>-1.1251925371151827E-3</v>
       </c>
       <c r="M6">
-        <f t="shared" si="5"/>
-        <v>461.33333333333394</v>
+        <f t="shared" si="6"/>
+        <v>1.8729205978690544E-2</v>
       </c>
       <c r="N6">
-        <f t="shared" si="6"/>
-        <v>-427.66666666666606</v>
+        <f t="shared" si="7"/>
+        <v>-1.7604013441575361E-2</v>
       </c>
       <c r="P6">
-        <f t="shared" si="7"/>
-        <v>1133.4444444444036</v>
+        <f t="shared" si="8"/>
+        <v>1.2660582455797018E-6</v>
       </c>
       <c r="Q6">
-        <f t="shared" si="8"/>
-        <v>212828.44444444499</v>
+        <f t="shared" si="9"/>
+        <v>3.5078315659221762E-4</v>
       </c>
       <c r="R6">
-        <f t="shared" si="9"/>
-        <v>182898.77777777726</v>
-      </c>
-    </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.2">
+        <f>N6^2</f>
+        <v>3.09901289251166E-4</v>
+      </c>
+      <c r="U6">
+        <f t="shared" si="11"/>
+        <v>3.0328976589642249E-3</v>
+      </c>
+      <c r="V6">
+        <f t="shared" si="12"/>
+        <v>1.2402618525327292E-3</v>
+      </c>
+      <c r="W6">
+        <f t="shared" si="13"/>
+        <v>5.119484210917972E-3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:24" x14ac:dyDescent="0.2">
       <c r="B7">
         <f>B3*$F3+B4*$F4+B5*$F5+B6*$F6</f>
-        <v>48189.666666666664</v>
+        <v>16.31855802918006</v>
       </c>
       <c r="C7">
-        <f t="shared" ref="C7:E7" si="10">C3*$F3+C4*$F4+C5*$F5+C6*$F6</f>
-        <v>-2364.3333333333339</v>
+        <f t="shared" ref="C7:E7" si="14">C3*$F3+C4*$F4+C5*$F5+C6*$F6</f>
+        <v>-8.7845849601839276E-2</v>
       </c>
       <c r="D7">
-        <f t="shared" si="10"/>
-        <v>-2065.0000000000036</v>
+        <f t="shared" si="14"/>
+        <v>-7.7207131742148327E-2</v>
       </c>
       <c r="E7">
-        <f t="shared" si="10"/>
-        <v>-1297.6666666666661</v>
+        <f t="shared" si="14"/>
+        <v>-5.0733248903462425E-2</v>
       </c>
       <c r="O7">
         <f>SUM(L3:N6)</f>
-        <v>1.8189894035458565E-12</v>
+        <v>-8.8817841970012523E-16</v>
       </c>
       <c r="R7" t="s">
         <v>10</v>
       </c>
       <c r="S7">
         <f>SUM(P3:R6)</f>
-        <v>876248</v>
-      </c>
-    </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.2">
+        <v>1.2471585744815979E-3</v>
+      </c>
+      <c r="X7">
+        <f>SUM(U3:W6)</f>
+        <v>1.3435931345796012E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:24" x14ac:dyDescent="0.2">
       <c r="B8">
         <f>B7/4</f>
-        <v>12047.416666666666</v>
+        <v>4.0796395072950151</v>
       </c>
       <c r="C8">
-        <f t="shared" ref="C8:E8" si="11">C7/4</f>
-        <v>-591.08333333333348</v>
+        <f t="shared" ref="C8:E8" si="15">C7/4</f>
+        <v>-2.1961462400459819E-2</v>
       </c>
       <c r="D8">
-        <f t="shared" si="11"/>
-        <v>-516.25000000000091</v>
+        <f t="shared" si="15"/>
+        <v>-1.9301782935537082E-2</v>
       </c>
       <c r="E8">
-        <f t="shared" si="11"/>
-        <v>-324.41666666666652</v>
-      </c>
-    </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.2">
+        <f t="shared" si="15"/>
+        <v>-1.2683312225865606E-2</v>
+      </c>
+      <c r="J8">
+        <f>AVERAGE(H3:J6)</f>
+        <v>4.0796395072950151</v>
+      </c>
+    </row>
+    <row r="9" spans="1:24" x14ac:dyDescent="0.2">
       <c r="C9">
         <f>POWER(C8,2)*4</f>
-        <v>1397518.0277777785</v>
+        <v>1.9292233230672415E-3</v>
       </c>
       <c r="D9">
-        <f t="shared" ref="D9:E9" si="12">POWER(D8,2)*4</f>
-        <v>1066056.2500000037</v>
+        <f t="shared" ref="D9:E9" si="16">POWER(D8,2)*4</f>
+        <v>1.4902352979623619E-3</v>
       </c>
       <c r="E9">
-        <f t="shared" si="12"/>
-        <v>420984.69444444403</v>
+        <f t="shared" si="16"/>
+        <v>6.4346563607516787E-4</v>
       </c>
       <c r="F9">
         <f>SUM(C9:E9)</f>
-        <v>2884558.9722222262</v>
-      </c>
-    </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.2">
+        <v>4.0629242571047714E-3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:24" x14ac:dyDescent="0.2">
       <c r="C10">
         <f>C9/$F$9</f>
-        <v>0.48448239097748413</v>
+        <v>0.4748361527275925</v>
       </c>
       <c r="D10">
-        <f t="shared" ref="D10:E10" si="13">D9/$F$9</f>
-        <v>0.36957339415346674</v>
+        <f t="shared" ref="D10:E10" si="17">D9/$F$9</f>
+        <v>0.36678884558490377</v>
       </c>
       <c r="E10">
-        <f t="shared" si="13"/>
-        <v>0.1459442148690491</v>
-      </c>
-    </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.2">
+        <f t="shared" si="17"/>
+        <v>0.15837500168750371</v>
+      </c>
+    </row>
+    <row r="12" spans="1:24" x14ac:dyDescent="0.2">
       <c r="I12" t="s">
         <v>10</v>
       </c>
       <c r="J12">
         <f>SUM(P3:R6)</f>
-        <v>876248</v>
+        <v>1.2471585744815979E-3</v>
       </c>
       <c r="K12">
         <f>J12/J18</f>
-        <v>9.1946999337583532E-2</v>
-      </c>
-    </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.2">
+        <v>9.2822636732992306E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:24" x14ac:dyDescent="0.2">
       <c r="I13" t="s">
         <v>12</v>
       </c>
       <c r="J13">
         <f>SUMSQ(H3:J6)</f>
-        <v>1751212905</v>
-      </c>
-    </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.2">
+        <v>199.73493804513359</v>
+      </c>
+    </row>
+    <row r="14" spans="1:24" x14ac:dyDescent="0.2">
       <c r="I14" t="s">
         <v>13</v>
       </c>
       <c r="J14">
         <f>4*3*B8^2</f>
-        <v>1741682980.083333</v>
-      </c>
-    </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.2">
+        <v>199.72150211378778</v>
+      </c>
+    </row>
+    <row r="15" spans="1:24" x14ac:dyDescent="0.2">
       <c r="I15" t="s">
         <v>14</v>
       </c>
       <c r="J15" s="1">
         <f>4*3*C8^2</f>
-        <v>4192554.0833333354</v>
+        <v>5.7876699692017246E-3</v>
       </c>
       <c r="K15">
         <f>J15/J18</f>
-        <v>0.43993568889519097</v>
-      </c>
-    </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.2">
+        <v>0.43076060901474988</v>
+      </c>
+    </row>
+    <row r="16" spans="1:24" x14ac:dyDescent="0.2">
       <c r="I16" t="s">
         <v>15</v>
       </c>
       <c r="J16" s="1">
         <f>4*3*D8^2</f>
-        <v>3198168.7500000112</v>
+        <v>4.470705893887086E-3</v>
       </c>
       <c r="K16">
         <f>J16/J18</f>
-        <v>0.33559222952603757</v>
+        <v>0.33274253781306284</v>
       </c>
     </row>
     <row r="17" spans="9:11" x14ac:dyDescent="0.2">
@@ -812,11 +869,11 @@
       </c>
       <c r="J17" s="1">
         <f>4*3*E8^2</f>
-        <v>1262954.0833333321</v>
+        <v>1.9303969082255035E-3</v>
       </c>
       <c r="K17">
         <f>J17/J18</f>
-        <v>0.13252508224115581</v>
+        <v>0.14367421643810485</v>
       </c>
     </row>
     <row r="18" spans="9:11" x14ac:dyDescent="0.2">
@@ -825,7 +882,7 @@
       </c>
       <c r="J18" s="1">
         <f>J13-J14</f>
-        <v>9529924.9166669846</v>
+        <v>1.3435931345810559E-2</v>
       </c>
     </row>
   </sheetData>
@@ -835,10 +892,117 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G4" sqref="E1:G4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1">
+        <v>12833</v>
+      </c>
+      <c r="B1">
+        <v>12684</v>
+      </c>
+      <c r="C1">
+        <v>12974</v>
+      </c>
+      <c r="E1">
+        <f>LOG10(A1)</f>
+        <v>4.1083281942661838</v>
+      </c>
+      <c r="F1">
+        <f t="shared" ref="F1:G1" si="0">LOG10(B1)</f>
+        <v>4.1032562333550509</v>
+      </c>
+      <c r="G1">
+        <f t="shared" si="0"/>
+        <v>4.1130738935942075</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>12732</v>
+      </c>
+      <c r="B2">
+        <v>12038</v>
+      </c>
+      <c r="C2">
+        <v>12121</v>
+      </c>
+      <c r="E2">
+        <f t="shared" ref="E2:E4" si="1">LOG10(A2)</f>
+        <v>4.1048966299489651</v>
+      </c>
+      <c r="F2">
+        <f t="shared" ref="F2:F4" si="2">LOG10(B2)</f>
+        <v>4.0805543389887715</v>
+      </c>
+      <c r="G2">
+        <f t="shared" ref="G2:G4" si="3">LOG10(C2)</f>
+        <v>4.0835384512301394</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>12140</v>
+      </c>
+      <c r="B3">
+        <v>12667</v>
+      </c>
+      <c r="C3">
+        <v>12533</v>
+      </c>
+      <c r="E3">
+        <f t="shared" si="1"/>
+        <v>4.0842186867392387</v>
+      </c>
+      <c r="F3">
+        <f t="shared" si="2"/>
+        <v>4.1026737705489271</v>
+      </c>
+      <c r="G3">
+        <f t="shared" si="3"/>
+        <v>4.0980550396692434</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>10582</v>
+      </c>
+      <c r="B4">
+        <v>11077</v>
+      </c>
+      <c r="C4">
+        <v>10188</v>
+      </c>
+      <c r="E4">
+        <f t="shared" si="1"/>
+        <v>4.0245677571960377</v>
+      </c>
+      <c r="F4">
+        <f t="shared" si="2"/>
+        <v>4.0444221557118434</v>
+      </c>
+      <c r="G4">
+        <f t="shared" si="3"/>
+        <v>4.0080889362915775</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:R8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K24" sqref="K24"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1156,7 +1320,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:Y6"/>
   <sheetViews>

</xml_diff>